<commit_message>
- Add feature to allow collection of more than 1 form per session - Updating Trackings
</commit_message>
<xml_diff>
--- a/src/main/resources/samples/tracking_list_sample_1.xlsx
+++ b/src/main/resources/samples/tracking_list_sample_1.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="30" windowWidth="18045" windowHeight="9030"/>
+    <workbookView windowWidth="22335" windowHeight="12030"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36">
   <si>
     <t>code</t>
   </si>
@@ -42,33 +42,33 @@
     <t>list_forms</t>
   </si>
   <si>
-    <t>member_code</t>
-  </si>
-  <si>
-    <t>member_studycode</t>
-  </si>
-  <si>
-    <t>member_forms</t>
-  </si>
-  <si>
-    <t>member_visit_nr</t>
+    <t>subject_code</t>
+  </si>
+  <si>
+    <t>subject_stype</t>
+  </si>
+  <si>
+    <t>subject_forms</t>
+  </si>
+  <si>
+    <t>subject_visit_nr</t>
+  </si>
+  <si>
+    <t>E02</t>
   </si>
   <si>
     <t>Eligibility Follow-up</t>
   </si>
   <si>
+    <t>Individuals</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Follow-up </t>
+  </si>
+  <si>
     <t>DSS_SURVEY</t>
   </si>
   <si>
-    <t>E01</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Follow-up </t>
-  </si>
-  <si>
-    <t>Individuals</t>
-  </si>
-  <si>
     <t>Followup Cases 1</t>
   </si>
   <si>
@@ -78,73 +78,419 @@
     <t>CHETM1024001</t>
   </si>
   <si>
+    <t>Member</t>
+  </si>
+  <si>
+    <t>Eligv1, Form1, Form3</t>
+  </si>
+  <si>
     <t>KABOD1013005</t>
   </si>
   <si>
+    <t>Eligv1, Form1, Form4</t>
+  </si>
+  <si>
     <t>CHETM1025001</t>
   </si>
   <si>
+    <t>Eligv1, Form1, Form5</t>
+  </si>
+  <si>
     <t>KABOD1013006</t>
   </si>
   <si>
+    <t>Followup Cases 3</t>
+  </si>
+  <si>
+    <t>Eligv1, Form1, Form6</t>
+  </si>
+  <si>
     <t>MAKTC2043004</t>
   </si>
   <si>
+    <t>Eligv1, Form1, Form7</t>
+  </si>
+  <si>
     <t>MM1WC1026001</t>
   </si>
   <si>
+    <t>Eligv1, Form1, Form8</t>
+  </si>
+  <si>
     <t>DISCM3036001</t>
   </si>
   <si>
+    <t>Eligv1, Form1, Form9</t>
+  </si>
+  <si>
     <t>CHEOD1050001</t>
-  </si>
-  <si>
-    <t>Eligv1, Form1, Form3</t>
-  </si>
-  <si>
-    <t>Eligv1, Form1, Form4</t>
-  </si>
-  <si>
-    <t>Eligv1, Form1, Form5</t>
-  </si>
-  <si>
-    <t>Eligv1, Form1, Form6</t>
-  </si>
-  <si>
-    <t>Eligv1, Form1, Form7</t>
-  </si>
-  <si>
-    <t>Eligv1, Form1, Form8</t>
-  </si>
-  <si>
-    <t>Eligv1, Form1, Form9</t>
-  </si>
-  <si>
-    <t>Followup Cases 3</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+  <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+  </numFmts>
+  <fonts count="21">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -152,9 +498,251 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="12" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="17" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="21" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="17" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -162,11 +750,58 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="60% - Accent6" xfId="1" builtinId="52"/>
+    <cellStyle name="40% - Accent6" xfId="2" builtinId="51"/>
+    <cellStyle name="60% - Accent5" xfId="3" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="4" builtinId="49"/>
+    <cellStyle name="40% - Accent5" xfId="5" builtinId="47"/>
+    <cellStyle name="20% - Accent5" xfId="6" builtinId="46"/>
+    <cellStyle name="60% - Accent4" xfId="7" builtinId="44"/>
+    <cellStyle name="Accent5" xfId="8" builtinId="45"/>
+    <cellStyle name="40% - Accent4" xfId="9" builtinId="43"/>
+    <cellStyle name="Accent4" xfId="10" builtinId="41"/>
+    <cellStyle name="Linked Cell" xfId="11" builtinId="24"/>
+    <cellStyle name="40% - Accent3" xfId="12" builtinId="39"/>
+    <cellStyle name="60% - Accent2" xfId="13" builtinId="36"/>
+    <cellStyle name="Accent3" xfId="14" builtinId="37"/>
+    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
+    <cellStyle name="20% - Accent2" xfId="16" builtinId="34"/>
+    <cellStyle name="Accent2" xfId="17" builtinId="33"/>
+    <cellStyle name="40% - Accent1" xfId="18" builtinId="31"/>
+    <cellStyle name="Accent1" xfId="19" builtinId="29"/>
+    <cellStyle name="Comma[0]" xfId="20" builtinId="6"/>
+    <cellStyle name="Neutral" xfId="21" builtinId="28"/>
+    <cellStyle name="60% - Accent1" xfId="22" builtinId="32"/>
+    <cellStyle name="Bad" xfId="23" builtinId="27"/>
+    <cellStyle name="20% - Accent4" xfId="24" builtinId="42"/>
+    <cellStyle name="Total" xfId="25" builtinId="25"/>
+    <cellStyle name="Output" xfId="26" builtinId="21"/>
+    <cellStyle name="Currency" xfId="27" builtinId="4"/>
+    <cellStyle name="20% - Accent3" xfId="28" builtinId="38"/>
+    <cellStyle name="Note" xfId="29" builtinId="10"/>
+    <cellStyle name="Input" xfId="30" builtinId="20"/>
+    <cellStyle name="Heading 4" xfId="31" builtinId="19"/>
+    <cellStyle name="Calculation" xfId="32" builtinId="22"/>
+    <cellStyle name="Good" xfId="33" builtinId="26"/>
+    <cellStyle name="Heading 3" xfId="34" builtinId="18"/>
+    <cellStyle name="CExplanatory Text" xfId="35" builtinId="53"/>
+    <cellStyle name="60% - Accent3" xfId="36" builtinId="40"/>
+    <cellStyle name="Currency[0]" xfId="37" builtinId="7"/>
+    <cellStyle name="Heading 1" xfId="38" builtinId="16"/>
+    <cellStyle name="20% - Accent6" xfId="39" builtinId="50"/>
+    <cellStyle name="Title" xfId="40" builtinId="15"/>
+    <cellStyle name="Warning Text" xfId="41" builtinId="11"/>
+    <cellStyle name="20% - Accent1" xfId="42" builtinId="30"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9"/>
+    <cellStyle name="Heading 2" xfId="45" builtinId="17"/>
+    <cellStyle name="Comma" xfId="46" builtinId="3"/>
+    <cellStyle name="Check Cell" xfId="47" builtinId="23"/>
+    <cellStyle name="Percent" xfId="48" builtinId="5"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9"/>
 </styleSheet>
 </file>
 
@@ -175,10 +810,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr val="windowText" lastClr="232627"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr val="window" lastClr="FCFCFC"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -454,27 +1089,28 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr/>
   <dimension ref="A1:L9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="7.75" style="1" customWidth="1"/>
-    <col min="2" max="2" width="17.875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="11.75" style="1" customWidth="1"/>
+    <col min="1" max="1" width="7.74814814814815" style="1" customWidth="1"/>
+    <col min="2" max="2" width="17.8740740740741" style="1" customWidth="1"/>
+    <col min="3" max="3" width="11.7481481481481" style="1" customWidth="1"/>
     <col min="4" max="4" width="9" style="1"/>
-    <col min="5" max="5" width="14.25" style="1" customWidth="1"/>
+    <col min="5" max="5" width="14.2518518518519" style="1" customWidth="1"/>
     <col min="6" max="6" width="9" style="1"/>
-    <col min="7" max="7" width="15.125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="17.25" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.125" style="1" customWidth="1"/>
-    <col min="10" max="10" width="20.125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="15.1259259259259" style="1" customWidth="1"/>
+    <col min="8" max="8" width="17.2518518518519" style="1" customWidth="1"/>
+    <col min="9" max="9" width="16.1259259259259" style="1" customWidth="1"/>
+    <col min="10" max="10" width="20.1259259259259" style="1" customWidth="1"/>
     <col min="11" max="11" width="18" style="1" customWidth="1"/>
-    <col min="12" max="12" width="17.625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="17.6222222222222" style="1" customWidth="1"/>
     <col min="13" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
@@ -518,19 +1154,19 @@
     </row>
     <row r="2" spans="1:12">
       <c r="A2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>14</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>16</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>15</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="F2" s="1">
         <v>1</v>
@@ -543,6 +1179,9 @@
       </c>
       <c r="I2" s="1" t="s">
         <v>19</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>20</v>
       </c>
       <c r="K2" s="1" t="s">
         <v>18</v>
@@ -553,19 +1192,19 @@
     </row>
     <row r="3" spans="1:12">
       <c r="A3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>14</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>16</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>15</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="F3" s="1">
         <v>1</v>
@@ -574,13 +1213,16 @@
         <v>17</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="I3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="J3" s="1" t="s">
         <v>20</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="L3" s="1">
         <v>1</v>
@@ -588,19 +1230,19 @@
     </row>
     <row r="4" spans="1:12">
       <c r="A4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>14</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>16</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>15</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="F4" s="1">
         <v>1</v>
@@ -609,13 +1251,16 @@
         <v>17</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>21</v>
+        <v>24</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>20</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="L4" s="1">
         <v>1</v>
@@ -623,19 +1268,19 @@
     </row>
     <row r="5" spans="1:12">
       <c r="A5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>14</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>16</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>15</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="F5" s="1">
         <v>1</v>
@@ -644,13 +1289,16 @@
         <v>17</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>22</v>
+        <v>26</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>20</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="L5" s="1">
         <v>1</v>
@@ -658,34 +1306,37 @@
     </row>
     <row r="6" spans="1:12">
       <c r="A6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>14</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>16</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>15</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="F6" s="1">
         <v>2</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>23</v>
+        <v>29</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>20</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="L6" s="1">
         <v>1</v>
@@ -693,34 +1344,37 @@
     </row>
     <row r="7" spans="1:12">
       <c r="A7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>14</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>16</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>15</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="F7" s="1">
         <v>2</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="H7" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="I7" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="I7" s="1" t="s">
-        <v>24</v>
+      <c r="J7" s="1" t="s">
+        <v>20</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="L7" s="1">
         <v>1</v>
@@ -728,31 +1382,34 @@
     </row>
     <row r="8" spans="1:12">
       <c r="A8" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>14</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>16</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>15</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="F8" s="1">
         <v>2</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="H8" s="1" t="s">
         <v>32</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>25</v>
+        <v>33</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>20</v>
       </c>
       <c r="K8" s="1" t="s">
         <v>32</v>
@@ -763,65 +1420,77 @@
     </row>
     <row r="9" spans="1:12">
       <c r="A9" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>14</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>16</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>15</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="F9" s="1">
         <v>2</v>
       </c>
       <c r="G9" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="H9" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="H9" s="1" t="s">
-        <v>33</v>
-      </c>
       <c r="I9" s="1" t="s">
-        <v>26</v>
+        <v>35</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>20</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="L9" s="1">
         <v>1</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="1" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr/>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75"/>
   <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr/>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75"/>
   <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>